<commit_message>
correccion de errores breves en el testing report
</commit_message>
<xml_diff>
--- a/reports/Student#2/hipothesis-contrast-july.xlsx
+++ b/reports/Student#2/hipothesis-contrast-july.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34692\Documents\CARRERA\4\2-cuatrimestre\DP2\JULIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34692\Documents\CARRERA\4\2-cuatrimestre\DP2\Workspace-DP2\Workspace-25\Projects\Acme-ANS-D04\reports\Student#2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DA256A-95AC-42E4-9E7B-0CE4B23DBC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8EA3DE-B8CB-42F2-B884-52FD2BA5C6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -178,15 +178,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -468,131 +466,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BAD935-C280-4EB0-8BB9-AA8127BDD507}">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="33.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>30.127791834170871</v>
-      </c>
-      <c r="C4" s="3">
-        <v>13.557000502512571</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1297.347438</v>
-      </c>
-      <c r="C5" s="3">
-        <v>180.96705879999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="3">
-        <v>796</v>
-      </c>
-      <c r="C6" s="3">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="3">
-        <v>12.159518126290944</v>
-      </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1.6448536269514715</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="4">
-        <v>1.9599639845400536</v>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J797"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -7203,4 +7080,120 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BAD935-C280-4EB0-8BB9-AA8127BDD507}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>30.127791834170871</v>
+      </c>
+      <c r="C4">
+        <v>13.557000502512571</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>1297.347438</v>
+      </c>
+      <c r="C5">
+        <v>180.96705879999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>796</v>
+      </c>
+      <c r="C6">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>12.159518126290944</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>1.6448536269514715</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.9599639845400536</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>